<commit_message>
Fix Comment text Getting...
</commit_message>
<xml_diff>
--- a/ClosedXML_Sandbox/test.xlsx
+++ b/ClosedXML_Sandbox/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ClosedXML\ClosedXML_Sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Repos\ClosedXML\ClosedXML_Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25128" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,64 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>adm-Knight, Andrew</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>adm-Knight, Andrew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+a comment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>adm-Knight, Andrew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+* A comment</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38,14 +96,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,8 +145,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -163,6 +262,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -198,6 +314,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -349,29 +482,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>